<commit_message>
Fix Givens QR on deflated sub-matrices
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/GivensQRTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/GivensQRTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="-165" windowWidth="14505" windowHeight="8130" activeTab="6"/>
+    <workbookView xWindow="1125" yWindow="-165" windowWidth="23775" windowHeight="12525" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="4x4(1)" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,16 @@
     <sheet name="5x5(1)" sheetId="6" r:id="rId5"/>
     <sheet name="5x5(2)" sheetId="7" r:id="rId6"/>
     <sheet name="5x5(3)" sheetId="8" r:id="rId7"/>
-    <sheet name="rand" sheetId="3" r:id="rId8"/>
+    <sheet name="4x4 in 6x6" sheetId="9" r:id="rId8"/>
+    <sheet name="4x4 in 6x6 Partial" sheetId="10" r:id="rId9"/>
+    <sheet name="rand" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="21">
   <si>
     <t>#0</t>
   </si>
@@ -73,15 +75,35 @@
   <si>
     <t xml:space="preserve">G1^t * G2^t * G3^t * G4^t = </t>
   </si>
+  <si>
+    <t>G1=</t>
+  </si>
+  <si>
+    <t>G2=</t>
+  </si>
+  <si>
+    <t>G3=</t>
+  </si>
+  <si>
+    <t>G3*G2*G1=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,13 +126,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1182,6 +1207,621 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f ca="1">RAND()*100 - 50</f>
+        <v>-13.972977432403546</v>
+      </c>
+      <c r="B1">
+        <f t="shared" ref="B1:G16" ca="1" si="0">RAND()*100 - 50</f>
+        <v>4.5676682268589346</v>
+      </c>
+      <c r="C1">
+        <f t="shared" ca="1" si="0"/>
+        <v>20.082176311918388</v>
+      </c>
+      <c r="D1">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.53969705499466158</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.5132419857542061</v>
+      </c>
+      <c r="F1">
+        <f t="shared" ca="1" si="0"/>
+        <v>29.686724622383423</v>
+      </c>
+      <c r="G1">
+        <f t="shared" ca="1" si="0"/>
+        <v>-31.531987070124813</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f t="shared" ref="A2:G20" ca="1" si="1">RAND()*100 - 50</f>
+        <v>-10.440501437285576</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ca="1" si="0"/>
+        <v>21.855147231623448</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ca="1" si="0"/>
+        <v>-39.430244101766547</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.2971348727406919</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.6561755331201198</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>47.2409690660715</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.9204263573896654</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ca="1" si="1"/>
+        <v>-41.129616609592347</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-42.274584543861629</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>31.072706492982391</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-16.830144600793219</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.3830303509623718</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-36.224116436501042</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-32.703565084828341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="1"/>
+        <v>-47.177859635665101</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.6061693690510097</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-27.023552481393342</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>23.242673513214086</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>36.592560380655073</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>43.396101881886608</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-25.274776369454333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="1"/>
+        <v>-8.3352317681634673</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>18.363137139904154</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>43.455902910899809</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-23.160596776911767</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-46.74709572547043</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>42.897198534744049</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>17.670860944079863</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="1"/>
+        <v>-11.680222674817657</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>32.603611352145435</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-18.362109659208635</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45.549366762793568</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-41.700325392883272</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>41.634951012994094</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>26.160054142660115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="1"/>
+        <v>-24.86204296278466</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-40.289798980468845</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>19.258870937844776</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-27.668688521022279</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>43.026325345900119</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-13.291815085108617</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-28.03040776108363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="1"/>
+        <v>-26.818320387523052</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-43.727918310061483</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-11.598748297501594</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>22.540581056648733</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-16.548593222175789</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-33.479729586811786</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-35.943292362488251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="1"/>
+        <v>-28.495648626489579</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.96683173215683382</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>13.119773002928881</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-8.2420591359668691</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-38.119276979833785</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-17.462060177798108</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="0"/>
+        <v>42.505480115122012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.82606198184159</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-39.713126826322025</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7444192975929695</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-49.238349692542585</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.919264648644095</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-38.104885506483967</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="0"/>
+        <v>34.330750641798275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" ca="1" si="1"/>
+        <v>40.313537108168333</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>41.591260402709622</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="0"/>
+        <v>16.009812681339426</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="0"/>
+        <v>43.611057240169345</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-26.446244169904965</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-37.026960003505771</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-36.060468867277372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ca="1" si="1"/>
+        <v>29.646537396816527</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>18.301625057083598</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-19.97235592520995</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-36.523033611729502</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-19.620401426395652</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>37.843173886161736</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.3292782102949303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.851230440761753</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-41.112463556318936</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-33.528412411889839</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="0"/>
+        <v>47.498333141359595</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.874419436756696</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>15.914974796126074</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-18.876386905829978</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" ca="1" si="1"/>
+        <v>45.190329049433444</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>28.060637210815457</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="0"/>
+        <v>38.607354899609675</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="0"/>
+        <v>27.553309360645471</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>-24.678915169210892</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>31.310512255844088</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="0"/>
+        <v>36.457333980289192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" ca="1" si="1"/>
+        <v>49.975368461659144</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-40.933387189358513</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-21.791066174880093</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="0"/>
+        <v>26.751409512769598</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="0"/>
+        <v>37.50483520874235</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-42.646274665857817</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="0"/>
+        <v>20.261885281969555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" ca="1" si="1"/>
+        <v>-12.721388617417198</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-8.7640117249135017</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-27.649065886666556</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-29.688027955644849</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.5490971096649986</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>12.178747812585023</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ca="1" si="0"/>
+        <v>45.782186703780027</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ca="1" si="1"/>
+        <v>18.479021504698522</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="1"/>
+        <v>-30.756715795685796</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4477363872106537</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>-39.423617497923267</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="1"/>
+        <v>-29.297424622311318</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="1"/>
+        <v>38.859862169807386</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ca="1" si="1"/>
+        <v>47.890329981093331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" ca="1" si="1"/>
+        <v>25.817825890542494</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="1"/>
+        <v>-24.350100271968923</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="1"/>
+        <v>-46.712936266286185</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="1"/>
+        <v>11.551215698396469</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="1"/>
+        <v>42.486566272131682</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.8719243336783222</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="1"/>
+        <v>-31.711628793331727</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" ca="1" si="1"/>
+        <v>17.499913188589133</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="1"/>
+        <v>31.583344357902945</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="1"/>
+        <v>-6.4703065180375248</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="1"/>
+        <v>-27.843785233925743</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>-24.626417458504879</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="1"/>
+        <v>33.625700504536894</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="1"/>
+        <v>-31.235279818333062</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-40.637499253910079</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.7486545730426712</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="1"/>
+        <v>14.284178132954253</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.687592434500615</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-16.602305839632614</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="1"/>
+        <v>31.860742058465291</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.028991728904785</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
@@ -2760,7 +3400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="D22" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
@@ -3547,7 +4187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -6126,7 +6766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -7427,612 +8067,2561 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <f ca="1">RAND()*100 - 50</f>
-        <v>11.138340056305992</v>
-      </c>
-      <c r="B1">
-        <f t="shared" ref="B1:G16" ca="1" si="0">RAND()*100 - 50</f>
-        <v>-24.535851448179891</v>
-      </c>
-      <c r="C1">
-        <f t="shared" ca="1" si="0"/>
-        <v>-16.402020109619627</v>
-      </c>
-      <c r="D1">
-        <f t="shared" ca="1" si="0"/>
-        <v>-3.3771674539137351</v>
-      </c>
-      <c r="E1">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.4161463713404814</v>
-      </c>
-      <c r="F1">
-        <f t="shared" ca="1" si="0"/>
-        <v>-9.7850996605667788</v>
-      </c>
-      <c r="G1">
-        <f t="shared" ca="1" si="0"/>
-        <v>-36.720081460323463</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:G20" ca="1" si="1">RAND()*100 - 50</f>
-        <v>4.6558908164744182</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <f t="shared" ca="1" si="0"/>
-        <v>40.549884884125589</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-24.870256076632614</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ca="1" si="0"/>
-        <v>47.822780786814121</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-38.438228252768084</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-44.466483277624356</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ca="1" si="0"/>
-        <v>40.882732697199501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.82524676356909055</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ca="1" si="0"/>
-        <v>-18.640066489858988</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ca="1" si="0"/>
-        <v>-44.374371527528297</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ca="1" si="0"/>
-        <v>-18.430618755675454</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>29.661455492155213</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>-24.151415550954582</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3652316715919568</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" ca="1" si="1"/>
-        <v>-47.016599989384233</v>
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>-34.028634392374848</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-35.081944023811353</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.3959041774840131</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-36.398416222229145</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8.5147158405827952</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-23.19528256019845</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.1915544907020035</v>
+        <v>49.910231472771827</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>-22.83304113392748</v>
+        <v>43.508124154091405</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="0"/>
-        <v>-41.094709437790101</v>
+        <v>18.905384002901187</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>-8.0058811970832977</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>14.160140566346996</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>40.987471397990788</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.7992357463405142</v>
+        <v>27.088576989338947</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12.485406702170835</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f>SQRT(B4*B4+B5*B5)</f>
+        <v>54.888518079427278</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <f>B4/H4</f>
+        <v>0.90930185800513785</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>J4</f>
+        <v>0.90930185800513785</v>
+      </c>
+      <c r="N4">
+        <f>-M5</f>
+        <v>0.41613715410715729</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>25.448644321591104</v>
+        <v>22.84115170673212</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>32.923236458230846</v>
+        <v>13.20688202784315</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>-32.30818558797499</v>
+        <v>20.881826975753626</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>-19.286154042348514</v>
+        <v>8.2717283527134029</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-35.179611068100435</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <f>-B5/H4</f>
+        <v>-0.41613715410715729</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>J5</f>
+        <v>-0.41613715410715729</v>
+      </c>
+      <c r="N5">
+        <f>M4</f>
+        <v>0.90930185800513785</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>-39.840435422989927</v>
+      </c>
+      <c r="D6">
+        <v>25.451029531712592</v>
+      </c>
+      <c r="E6">
+        <v>-37.315259039343296</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.6501593692368886</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>14.386082400805094</v>
+      </c>
+      <c r="E7">
+        <v>-17.097446277781657</v>
+      </c>
+      <c r="F7" s="1">
+        <v>17.279169789255121</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-15.681027926373091</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="array" ref="A12:F17">MMULT(L3:Q8,A3:F8)</f>
+        <v>-34.028634392374848</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-35.081944023811353</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.3959041774840131</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-36.398416222229145</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8.5147158405827952</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-23.19528256019845</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>54.888518079427271</v>
+      </c>
+      <c r="C13">
+        <v>45.057892433329144</v>
+      </c>
+      <c r="D13">
+        <v>25.880404850386842</v>
+      </c>
+      <c r="E13">
+        <v>28.073866883366769</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-3.2865397202422262</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>-6.0963045996520275</v>
+      </c>
+      <c r="D14">
+        <v>11.120651371324303</v>
+      </c>
+      <c r="E14">
+        <v>-3.7510653771200602</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-37.184527321033634</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <f>SQRT(C14*C14+C15*C15)</f>
+        <v>40.304158897875155</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f>C14/H14</f>
+        <v>-0.15125745745244731</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>J14</f>
+        <v>-0.15125745745244731</v>
+      </c>
+      <c r="O14">
+        <f>-N15</f>
+        <v>-0.98849440138273981</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>-39.840435422989927</v>
+      </c>
+      <c r="D15">
+        <v>25.451029531712592</v>
+      </c>
+      <c r="E15">
+        <v>-37.315259039343296</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.6501593692368886</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <f>-C15/H14</f>
+        <v>0.98849440138273981</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f>J15</f>
+        <v>0.98849440138273981</v>
+      </c>
+      <c r="O15">
+        <f>N14</f>
+        <v>-0.15125745745244731</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>14.386082400805094</v>
+      </c>
+      <c r="E16">
+        <v>-17.097446277781657</v>
+      </c>
+      <c r="F16" s="1">
+        <v>17.279169789255121</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-15.681027926373091</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="L20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="array" ref="A21:F26">MMULT(L12:Q17,A12:F17)</f>
+        <v>-34.028634392374848</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-35.081944023811353</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2.3959041774840131</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-36.398416222229145</v>
+      </c>
+      <c r="E21" s="1">
+        <v>8.5147158405827952</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-23.19528256019845</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>54.888518079427271</v>
+      </c>
+      <c r="C22">
+        <v>45.057892433329144</v>
+      </c>
+      <c r="D22">
+        <v>25.880404850386842</v>
+      </c>
+      <c r="E22">
+        <v>28.073866883366769</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-3.2865397202422262</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>40.304158897875155</v>
+      </c>
+      <c r="D23">
+        <v>-26.840281653166258</v>
+      </c>
+      <c r="E23">
+        <v>37.453301258218609</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3.9932637612706725</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>7.1430436037693639</v>
+      </c>
+      <c r="E24">
+        <v>1.9363040819667034</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-37.006295985487384</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <f>SQRT(D24*D24+D25*D25)</f>
+        <v>16.06183173763517</v>
+      </c>
+      <c r="I24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <f>D24/H24</f>
+        <v>0.44472160588211057</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>J24</f>
+        <v>0.44472160588211057</v>
+      </c>
+      <c r="P24">
+        <f>-O25</f>
+        <v>0.89566885245699868</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>14.386082400805094</v>
+      </c>
+      <c r="E25">
+        <v>-17.097446277781657</v>
+      </c>
+      <c r="F25" s="1">
+        <v>17.279169789255121</v>
+      </c>
+      <c r="I25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <f>-D25/H24</f>
+        <v>-0.89566885245699868</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>J25</f>
+        <v>-0.89566885245699868</v>
+      </c>
+      <c r="P25">
+        <f>O24</f>
+        <v>0.44472160588211057</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>-15.681027926373091</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="L29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="array" ref="A30:F35">MMULT(L21:Q26,A21:F26)</f>
+        <v>-34.028634392374848</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-35.081944023811353</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2.3959041774840131</v>
+      </c>
+      <c r="D30" s="1">
+        <v>-36.398416222229145</v>
+      </c>
+      <c r="E30" s="1">
+        <v>8.5147158405827952</v>
+      </c>
+      <c r="F30" s="1">
+        <v>-23.19528256019845</v>
+      </c>
+      <c r="L30">
+        <f t="array" ref="L30:Q35">MMULT(L21:Q26,MMULT(L12:Q17,L3:Q8))</f>
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>54.888518079427271</v>
+      </c>
+      <c r="C31">
+        <v>45.057892433329144</v>
+      </c>
+      <c r="D31">
+        <v>25.880404850386842</v>
+      </c>
+      <c r="E31">
+        <v>28.073866883366769</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-3.2865397202422262</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0.90930185800513785</v>
+      </c>
+      <c r="N31">
+        <v>0.41613715410715729</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>40.304158897875155</v>
+      </c>
+      <c r="D32">
+        <v>-26.840281653166258</v>
+      </c>
+      <c r="E32">
+        <v>37.453301258218609</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3.9932637612706725</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>6.2943847881745854E-2</v>
+      </c>
+      <c r="N32">
+        <v>-0.13753868709864342</v>
+      </c>
+      <c r="O32">
+        <v>-0.98849440138273981</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>16.061831737635174</v>
+      </c>
+      <c r="E33">
+        <v>-14.452533826757563</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-0.98108520186287507</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>-0.18293589772303595</v>
+      </c>
+      <c r="N33">
+        <v>0.39973347742114879</v>
+      </c>
+      <c r="O33">
+        <v>-6.7267459379897379E-2</v>
+      </c>
+      <c r="P33">
+        <v>0.89566885245699868</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>-8.8817841970012523E-16</v>
+      </c>
+      <c r="E34">
+        <v>-9.3378910202410914</v>
+      </c>
+      <c r="F34" s="1">
+        <v>40.82980679599271</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0.36843270805740169</v>
+      </c>
+      <c r="N34">
+        <v>-0.80506280845134903</v>
+      </c>
+      <c r="O34">
+        <v>0.1354765933419968</v>
+      </c>
+      <c r="P34">
+        <v>0.44472160588211057</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-15.681027926373091</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="array" ref="A39:F44">MMULT(A30:F35,TRANSPOSE(L30:Q35))</f>
+        <v>-34.028634392374848</v>
+      </c>
+      <c r="B39">
+        <v>-30.903052137352258</v>
+      </c>
+      <c r="C39">
+        <v>33.44190859185619</v>
+      </c>
+      <c r="D39">
+        <v>17.450264782952384</v>
+      </c>
+      <c r="E39">
+        <v>-15.998644317094447</v>
+      </c>
+      <c r="F39">
+        <v>-23.19528256019845</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>68.660494600043819</v>
+      </c>
+      <c r="C40">
+        <v>-28.324944136392158</v>
+      </c>
+      <c r="D40">
+        <v>31.374046751542565</v>
+      </c>
+      <c r="E40">
+        <v>-6.0463820880137575E-2</v>
+      </c>
+      <c r="F40">
+        <v>-3.2865397202422262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>16.772057982444426</v>
+      </c>
+      <c r="C41">
+        <v>20.988087046261857</v>
+      </c>
+      <c r="D41">
+        <v>51.462154505306458</v>
+      </c>
+      <c r="E41">
+        <v>-19.427316996162006</v>
+      </c>
+      <c r="F41">
+        <v>3.9932637612706725</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>-15.877030748603973</v>
+      </c>
+      <c r="D42">
+        <v>-14.025123001686023</v>
+      </c>
+      <c r="E42">
+        <v>-4.2513518058539699</v>
+      </c>
+      <c r="F42">
+        <v>-0.98108520186287507</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>8.7795939530254313E-16</v>
+      </c>
+      <c r="D43">
+        <v>-8.3636581344678511</v>
+      </c>
+      <c r="E43">
+        <v>-4.1527618900737577</v>
+      </c>
+      <c r="F43">
+        <v>40.82980679599271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>-15.681027926373091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>32.294327963090765</v>
+      </c>
+      <c r="B3" s="1">
+        <v>16.067058615351513</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-16.56437078489644</v>
+      </c>
+      <c r="D3" s="1">
+        <v>37.606350204367018</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-0.70684404915649424</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.5781209892427484</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>19.492037142846229</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-17.78193604217082</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-44.656480460169711</v>
+      </c>
+      <c r="E4" s="1">
+        <v>13.187804104130599</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12.731814755750278</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-12.498724934625137</v>
+      </c>
+      <c r="D5">
+        <v>38.977757825536997</v>
+      </c>
+      <c r="E5">
+        <v>34.142740580850784</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>-29.751562068818771</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.5632351339004202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" ca="1" si="1"/>
-        <v>14.079971619917288</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ca="1" si="0"/>
-        <v>49.144496397967771</v>
+        <v>10.215530967667974</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f>SQRT(C5*C5+C6*C6)</f>
+        <v>30.523364048163778</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f>C5/H5</f>
+        <v>-0.40948058395211634</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f>J5</f>
+        <v>-0.40948058395211634</v>
+      </c>
+      <c r="O5">
+        <f>-N6</f>
+        <v>-0.91231883207913334</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>48.998297366162831</v>
+        <v>-27.847039839546984</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>-33.670893146489092</v>
+        <v>24.248194619138488</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="0"/>
-        <v>15.827551665304426</v>
+        <v>-1.3367270175319277</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="0"/>
-        <v>-21.778989248866854</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.1517622375646894</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ca="1" si="1"/>
-        <v>29.252519109025712</v>
-      </c>
-      <c r="B7">
-        <f t="shared" ca="1" si="0"/>
-        <v>-25.176392953144099</v>
+        <v>45.276094801042049</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <f>-C6/H5</f>
+        <v>0.91231883207913334</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f>J6</f>
+        <v>0.91231883207913334</v>
+      </c>
+      <c r="O6">
+        <f>N5</f>
+        <v>-0.40948058395211634</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>-13.578135637476088</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>-49.370087088312708</v>
+        <v>-14.89813543421905</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>-9.2957800307686398</v>
+        <v>7.3453316366515082</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>11.087326259913922</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>38.000677900786513</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" ca="1" si="1"/>
-        <v>41.034276756774176</v>
-      </c>
-      <c r="B8">
-        <f t="shared" ca="1" si="0"/>
-        <v>-3.7439498208245681</v>
+        <v>16.880904157669278</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>-39.813872516530303</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="0"/>
-        <v>18.675200960594921</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>-28.717101763670662</v>
+        <v>-32.789626438039917</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>-14.639576608806991</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>29.648014099411625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" ca="1" si="1"/>
-        <v>-29.162697574575002</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>22.350381892764688</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5016197505929227</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ca="1" si="0"/>
-        <v>-13.507064405558246</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ca="1" si="0"/>
-        <v>11.108672714867275</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>24.691891947580785</v>
-      </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="0"/>
-        <v>-41.756394633044678</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" ca="1" si="1"/>
-        <v>-4.28942639665798</v>
-      </c>
-      <c r="B10">
-        <f t="shared" ca="1" si="0"/>
-        <v>43.373137979897862</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ca="1" si="0"/>
-        <v>-46.475394189965925</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>-2.3521027436113826</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8607778713661247</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.8406092012428985</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ca="1" si="0"/>
-        <v>-10.769805429852198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-31.401342868224667</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ca="1" si="1"/>
-        <v>-44.936236240002835</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="0"/>
-        <v>-25.445184593667548</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ca="1" si="0"/>
-        <v>-25.021872183744975</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>-1.8708086337807757</v>
-      </c>
-      <c r="E11">
-        <f t="shared" ca="1" si="0"/>
-        <v>48.291833367438713</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ca="1" si="0"/>
-        <v>-15.26772608578144</v>
-      </c>
-      <c r="G11">
-        <f t="shared" ca="1" si="0"/>
-        <v>12.460917502738852</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" ca="1" si="1"/>
-        <v>-33.088895244319083</v>
-      </c>
-      <c r="B12">
-        <f t="shared" ca="1" si="0"/>
-        <v>18.977207450657701</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ca="1" si="0"/>
-        <v>-32.46490258082153</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>-32.908704828879898</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ca="1" si="0"/>
-        <v>-7.169175979598073</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>-33.547770736865836</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="0"/>
-        <v>-48.221520843645962</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" ca="1" si="1"/>
-        <v>46.750413863389667</v>
-      </c>
-      <c r="B13">
-        <f t="shared" ca="1" si="0"/>
-        <v>-23.148080526048243</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ca="1" si="0"/>
-        <v>36.898893349305382</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ca="1" si="0"/>
-        <v>-7.7115739858574557</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ca="1" si="0"/>
-        <v>-11.79112369254053</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>-49.943127450751149</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>29.489073586802846</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" ca="1" si="1"/>
-        <v>26.022152335897474</v>
-      </c>
-      <c r="B14">
-        <f t="shared" ca="1" si="0"/>
-        <v>-26.484363085441764</v>
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="array" ref="A12:F17">MMULT(L3:Q8,A3:F8)</f>
+        <v>32.294327963090765</v>
+      </c>
+      <c r="B12" s="1">
+        <v>16.067058615351513</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-16.56437078489644</v>
+      </c>
+      <c r="D12" s="1">
+        <v>37.606350204367018</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-0.70684404915649424</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3.5781209892427484</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>19.492037142846229</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-17.78193604217082</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-44.656480460169711</v>
+      </c>
+      <c r="E13" s="1">
+        <v>13.187804104130599</v>
+      </c>
+      <c r="F13" s="1">
+        <v>12.731814755750278</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="0"/>
-        <v>-31.576772568068179</v>
+        <v>30.523364048163778</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2636418763885118</v>
+        <v>-38.082719630505011</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="0"/>
-        <v>-9.1390651575282789</v>
+        <v>-12.761268119329047</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>-1.1189066167636597</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="0"/>
-        <v>-20.870662568039055</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" ca="1" si="1"/>
-        <v>-3.9489866825327624</v>
-      </c>
-      <c r="B15">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.0083269899709038</v>
+        <v>-45.489295516012412</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.4440536453621249</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="0"/>
-        <v>11.23168648664813</v>
+        <v>25.630977604027819</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="0"/>
-        <v>29.393553106500235</v>
+        <v>31.696428970426162</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>34.682609288152236</v>
-      </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="0"/>
-        <v>-1.7544176346623743</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" ca="1" si="1"/>
-        <v>-45.766716287386934</v>
-      </c>
-      <c r="B16">
-        <f t="shared" ca="1" si="0"/>
-        <v>-35.343349502046109</v>
+        <v>-9.2198604567110127</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f>SQRT(D15*D15+D16*D16)</f>
+        <v>29.64627214936996</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <f>D15/H15</f>
+        <v>0.86455988378196569</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>J15</f>
+        <v>0.86455988378196569</v>
+      </c>
+      <c r="P15">
+        <f>-O16</f>
+        <v>-0.50252980742928466</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="0"/>
-        <v>-27.356163062588269</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="0"/>
-        <v>-7.617159392336383</v>
+        <v>-14.89813543421905</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.4838681380997585</v>
+        <v>7.3453316366515082</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>-15.161189684672962</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="0"/>
-        <v>12.797268818107767</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" ca="1" si="1"/>
-        <v>10.228299209365929</v>
-      </c>
-      <c r="B17">
-        <f t="shared" ca="1" si="1"/>
-        <v>22.091662905966444</v>
+        <v>16.880904157669278</v>
+      </c>
+      <c r="I16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <f>-D16/H15</f>
+        <v>0.50252980742928466</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>J16</f>
+        <v>0.50252980742928466</v>
+      </c>
+      <c r="P16">
+        <f>O15</f>
+        <v>0.86455988378196569</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="1"/>
-        <v>-11.841225520786715</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>-2.5025450052420268</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.87921141816251946</v>
+        <v>-32.789626438039917</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="1"/>
-        <v>36.082053328537526</v>
-      </c>
-      <c r="G17">
-        <f t="shared" ca="1" si="1"/>
-        <v>22.347516381539918</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" ca="1" si="1"/>
-        <v>27.077855576880864</v>
-      </c>
-      <c r="B18">
-        <f t="shared" ca="1" si="1"/>
-        <v>30.44195646832938</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ca="1" si="1"/>
-        <v>-32.187695808786884</v>
-      </c>
-      <c r="D18">
-        <f t="shared" ca="1" si="1"/>
-        <v>-2.6782923432875165</v>
-      </c>
-      <c r="E18">
-        <f t="shared" ca="1" si="1"/>
-        <v>20.961495624927863</v>
-      </c>
-      <c r="F18">
-        <f t="shared" ca="1" si="1"/>
-        <v>-10.161598025308408</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ca="1" si="1"/>
-        <v>47.516933137990407</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" ca="1" si="1"/>
-        <v>-9.8653470909723637</v>
-      </c>
-      <c r="B19">
-        <f t="shared" ca="1" si="1"/>
-        <v>-32.119376065117407</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ca="1" si="1"/>
-        <v>34.956518008243549</v>
-      </c>
-      <c r="D19">
-        <f t="shared" ca="1" si="1"/>
-        <v>-29.960315570763164</v>
-      </c>
-      <c r="E19">
-        <f t="shared" ca="1" si="1"/>
-        <v>-31.540108433335455</v>
-      </c>
-      <c r="F19">
-        <f t="shared" ca="1" si="1"/>
-        <v>40.801874713378666</v>
-      </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>11.930568263550065</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-31.401342868224667</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" ca="1" si="1"/>
-        <v>-6.3457783850028449</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="1"/>
-        <v>-2.478392098800029</v>
-      </c>
-      <c r="C20">
-        <f t="shared" ca="1" si="1"/>
-        <v>-46.330753811389172</v>
-      </c>
-      <c r="D20">
-        <f t="shared" ca="1" si="1"/>
-        <v>-47.944572774288275</v>
-      </c>
-      <c r="E20">
-        <f t="shared" ca="1" si="1"/>
-        <v>43.038061600610831</v>
-      </c>
-      <c r="F20">
-        <f t="shared" ca="1" si="1"/>
-        <v>10.221418173195062</v>
-      </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>28.931556506511797</v>
+        <v>6</v>
+      </c>
+      <c r="L20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="array" ref="A21:F26">MMULT(L12:Q17,A12:F17)</f>
+        <v>32.294327963090765</v>
+      </c>
+      <c r="B21" s="1">
+        <v>16.067058615351513</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-16.56437078489644</v>
+      </c>
+      <c r="D21" s="1">
+        <v>37.606350204367018</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-0.70684404915649424</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3.5781209892427484</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>19.492037142846229</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-17.78193604217082</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-44.656480460169711</v>
+      </c>
+      <c r="E22" s="1">
+        <v>13.187804104130599</v>
+      </c>
+      <c r="F22" s="1">
+        <v>12.731814755750278</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>30.523364048163778</v>
+      </c>
+      <c r="D23">
+        <v>-38.082719630505011</v>
+      </c>
+      <c r="E23">
+        <v>-12.761268119329047</v>
+      </c>
+      <c r="F23">
+        <v>-45.489295516012412</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>29.64627214936996</v>
+      </c>
+      <c r="E24">
+        <v>23.712212854104258</v>
+      </c>
+      <c r="F24">
+        <v>-16.454279000525766</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>22.278879412827681</v>
+      </c>
+      <c r="F25">
+        <v>9.9612978368531913</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <f>SQRT(E25*E25+E26*E26)</f>
+        <v>39.642251069250889</v>
+      </c>
+      <c r="I25" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <f>E25/H25</f>
+        <v>0.56199834297776874</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f>J25</f>
+        <v>0.56199834297776874</v>
+      </c>
+      <c r="Q25">
+        <f>-P26</f>
+        <v>-0.82713835752565745</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>-32.789626438039917</v>
+      </c>
+      <c r="F26">
+        <v>-31.401342868224667</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <f>-E26/H25</f>
+        <v>0.82713835752565745</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f>J26</f>
+        <v>0.82713835752565745</v>
+      </c>
+      <c r="Q26">
+        <f>P25</f>
+        <v>0.56199834297776874</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="L29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="array" ref="A30:F35">MMULT(L21:Q26,A21:F26)</f>
+        <v>32.294327963090765</v>
+      </c>
+      <c r="B30" s="1">
+        <v>16.067058615351513</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-16.56437078489644</v>
+      </c>
+      <c r="D30" s="1">
+        <v>37.606350204367018</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-0.70684404915649424</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3.5781209892427484</v>
+      </c>
+      <c r="L30">
+        <f t="array" ref="L30:Q35">MMULT(L21:Q26,MMULT(L12:Q17,L3:Q8))</f>
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>19.492037142846229</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-17.78193604217082</v>
+      </c>
+      <c r="D31" s="1">
+        <v>-44.656480460169711</v>
+      </c>
+      <c r="E31" s="1">
+        <v>13.187804104130599</v>
+      </c>
+      <c r="F31" s="1">
+        <v>12.731814755750278</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>30.523364048163778</v>
+      </c>
+      <c r="D32">
+        <v>-38.082719630505011</v>
+      </c>
+      <c r="E32">
+        <v>-12.761268119329047</v>
+      </c>
+      <c r="F32">
+        <v>-45.489295516012412</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>-0.40948058395211634</v>
+      </c>
+      <c r="O32">
+        <v>-0.91231883207913334</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>29.64627214936996</v>
+      </c>
+      <c r="E33">
+        <v>23.712212854104258</v>
+      </c>
+      <c r="F33">
+        <v>-16.454279000525766</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0.78875426343443422</v>
+      </c>
+      <c r="O33">
+        <v>-0.35402048607261316</v>
+      </c>
+      <c r="P33">
+        <v>-0.50252980742928466</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>39.642251069250889</v>
+      </c>
+      <c r="F34">
+        <v>31.571488042342896</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0.25765792304266055</v>
+      </c>
+      <c r="O34">
+        <v>-0.11564588286197587</v>
+      </c>
+      <c r="P34">
+        <v>0.48588122209051704</v>
+      </c>
+      <c r="Q34">
+        <v>-0.82713835752565745</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>-9.4081311276204058</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0.37921597800406492</v>
+      </c>
+      <c r="O35">
+        <v>-0.17020538725830939</v>
+      </c>
+      <c r="P35">
+        <v>0.71511064225398835</v>
+      </c>
+      <c r="Q35">
+        <v>0.56199834297776874</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="array" ref="A39:F44">MMULT(A30:F35,TRANSPOSE(L30:Q35))</f>
+        <v>32.294327963090765</v>
+      </c>
+      <c r="B39">
+        <v>16.067058615351513</v>
+      </c>
+      <c r="C39">
+        <v>-27.526193275408225</v>
+      </c>
+      <c r="D39">
+        <v>-26.023426252557631</v>
+      </c>
+      <c r="E39">
+        <v>-11.920004312047508</v>
+      </c>
+      <c r="F39">
+        <v>-11.176851102159665</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>19.492037142846229</v>
+      </c>
+      <c r="C40">
+        <v>48.022305652533959</v>
+      </c>
+      <c r="D40">
+        <v>-4.8435336034431105</v>
+      </c>
+      <c r="E40">
+        <v>-3.5405845705651631</v>
+      </c>
+      <c r="F40">
+        <v>17.443577141934949</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>22.244857361074281</v>
+      </c>
+      <c r="D41">
+        <v>43.97041405246884</v>
+      </c>
+      <c r="E41">
+        <v>43.694176947249154</v>
+      </c>
+      <c r="F41">
+        <v>-16.633795951955495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>-27.046852382813338</v>
+      </c>
+      <c r="D42">
+        <v>-22.411481435856146</v>
+      </c>
+      <c r="E42">
+        <v>21.702814950506145</v>
+      </c>
+      <c r="F42">
+        <v>2.6636229982236497</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>-19.921412795894003</v>
+      </c>
+      <c r="E43">
+        <v>-6.8525633680377105</v>
+      </c>
+      <c r="F43">
+        <v>46.091719587665011</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>7.781826128285954</v>
+      </c>
+      <c r="F44">
+        <v>-5.2873541042402348</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <f>A30</f>
+        <v>32.294327963090765</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" ref="B48:F49" si="0">B30</f>
+        <v>16.067058615351513</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="0"/>
+        <v>-16.56437078489644</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>37.606350204367018</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.70684404915649424</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5781209892427484</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <f>A31</f>
+        <v>0</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="0"/>
+        <v>19.492037142846229</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="0"/>
+        <v>-17.78193604217082</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>-44.656480460169711</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="0"/>
+        <v>13.187804104130599</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="0"/>
+        <v>12.731814755750278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f t="shared" ref="A50:F50" si="1">A41</f>
+        <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>22.244857361074281</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>43.97041405246884</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>43.694176947249154</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>-16.633795951955495</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <f t="shared" ref="A51:F51" si="2">A42</f>
+        <v>0</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>-27.046852382813338</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>-22.411481435856146</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>21.702814950506145</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>2.6636229982236497</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <f t="shared" ref="A52:F52" si="3">A43</f>
+        <v>0</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="3"/>
+        <v>-19.921412795894003</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="3"/>
+        <v>-6.8525633680377105</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>46.091719587665011</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <f t="shared" ref="A53:F53" si="4">A44</f>
+        <v>0</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="4"/>
+        <v>7.781826128285954</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="4"/>
+        <v>-5.2873541042402348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>